<commit_message>
updated evaluation with new sensotwin file
</commit_message>
<xml_diff>
--- a/requests.xlsx
+++ b/requests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jun\Desktop\materialdigital1_ontology_collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D823D2DA-1972-43DC-A8DC-07701911674D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4F5126-6480-47B9-A036-D5E10E1DD6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F127" sqref="F127"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>